<commit_message>
readme and input-output files updated with zenodo link
</commit_message>
<xml_diff>
--- a/scripts/scripts_functions_input_output.xlsx
+++ b/scripts/scripts_functions_input_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rosa\Documents\GitHub\forest-management\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8244DAB3-38F6-4196-B0F8-464672C3E8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9F2DA3-47A2-43B5-A79F-2CF376569A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1650" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3510" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output" sheetId="1" r:id="rId1"/>
@@ -564,6 +564,70 @@
       </rPr>
       <t>: the .csv files in data/model_parameters/ecoregions_data/ were used as input files but are  not owned by the authors for the manuscript but by the authors of the references listed in the readme.md in data/model_parameters/ecoregions_data.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">scripts/plotting/maps_shapefiles/WWF_Ecoregions/
+results/species-lost_*/Slost_year_*.csv
+* cutoff_static_Baseline, cutoff_static_SharedEffort, cutoff_static_LowerIntensity, cutoff_bs_Baseline, 
+cutoff_bs_SharedEffort, cutoff_timber_static_Baseline, according to the selected scenario.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IMPORTANT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: the folder WWF_Ecoregions and the relative shapefiles were not uploaded to github as they are not owned by the authors for the manuscript but by the authors of the reference listed in the readme.md in scripts/readme.md. In the readme.md file there is also a link to the page from where the shp of the ecoregions was downloaded.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data/model_parameters/ecoregions_data/z_analysis/z_SAR_data_full-table.csv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IMPORTANT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: this file was not uploaded to the github repo as it is not owned by the authors for the manuscript but by the authors of the reference listed in the readme.md in data/model_parameters/ecoregions_data/z_analysis.</t>
+    </r>
+  </si>
+  <si>
+    <t>data/model_parameters/ecoregions_data/Ecoregions_description.csv
+data/model_parameters/ecoregions_data/CF_local.csv
+data/model_parameters/ecoregions_data/CF_local_forest-use.csv
+data/model_parameters/ecoregions_data/z_input-values.csv
+Variables defined in the scripts where the functions are called.</t>
   </si>
   <si>
     <r>
@@ -596,7 +660,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: rr_ecoregion_bs.Rdata and zvalues_ecoregion_bs.Rdata (used in scripts/model/calculate_impacts.R  when the option to calculate the confidence intervals is on) were too big to be uploaded on github. Therefore, these files have been uploaded to zenodo. When the confidence intervals are not calculated, these files are not needed. </t>
+      <t xml:space="preserve">: rr_ecoregion_bs.Rdata and zvalues_ecoregion_bs.Rdata (used in scripts/model/calculate_impacts.R  when the option to calculate the confidence intervals is on) were too big to be uploaded on github. Therefore, these files have been uploaded to zenodo (https://zenodo.org/record/7543683#.Y9Vh-LXMJaQ). When the confidence intervals are not calculated, these files are not needed. </t>
     </r>
   </si>
   <si>
@@ -627,72 +691,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: rr_ecoregion_bs.Rdata and zvalues_ecoregion_bs.Rdata (used in scripts/model/calculate_impacts.R  when the option to calculate the confidence intervals is on) were too big to be uploaded on github. Therefore, these files have been uploaded to zenodo. When the confidence intervals are not calculated, these files are not needed. </t>
+      <t xml:space="preserve">: rr_ecoregion_bs.Rdata and zvalues_ecoregion_bs.Rdata (used in scripts/model/calculate_impacts.R  when the option to calculate the confidence intervals is on) were too big to be uploaded on github. Therefore, these files have been uploaded to zenodo (https://zenodo.org/record/7543683#.Y9Vh-LXMJaQ). When the confidence intervals are not calculated, these files are not needed. </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">scripts/plotting/maps_shapefiles/WWF_Ecoregions/
-results/species-lost_*/Slost_year_*.csv
-* cutoff_static_Baseline, cutoff_static_SharedEffort, cutoff_static_LowerIntensity, cutoff_bs_Baseline, 
-cutoff_bs_SharedEffort, cutoff_timber_static_Baseline, according to the selected scenario.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IMPORTANT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: the folder WWF_Ecoregions and the relative shapefiles were not uploaded to github as they are not owned by the authors for the manuscript but by the authors of the reference listed in the readme.md in scripts/readme.md. In the readme.md file there is also a link to the page from where the shp of the ecoregions was downloaded.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">data/model_parameters/ecoregions_data/z_analysis/z_SAR_data_full-table.csv
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IMPORTANT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: this file was not uploaded to the github repo as it is not owned by the authors for the manuscript but by the authors of the reference listed in the readme.md in data/model_parameters/ecoregions_data/z_analysis.</t>
-    </r>
-  </si>
-  <si>
-    <t>data/model_parameters/ecoregions_data/Ecoregions_description.csv
-data/model_parameters/ecoregions_data/CF_local.csv
-data/model_parameters/ecoregions_data/CF_local_forest-use.csv
-data/model_parameters/ecoregions_data/z_input-values.csv
-Variables defined in the scripts where the functions are called.</t>
   </si>
 </sst>
 </file>
@@ -1605,9 +1605,9 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.45"/>
@@ -1754,7 +1754,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>24</v>
@@ -1869,10 +1869,10 @@
         <v>44</v>
       </c>
       <c r="F11" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.45">
@@ -1938,7 +1938,7 @@
         <v>53</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>54</v>
@@ -2237,7 +2237,7 @@
         <v>17</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>105</v>
@@ -2260,7 +2260,7 @@
         <v>104</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>106</v>

</xml_diff>